<commit_message>
Correcciones, se agregaron más columnas
</commit_message>
<xml_diff>
--- a/src/archivo.xlsx
+++ b/src/archivo.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12640"/>
+    <workbookView xWindow="2520" yWindow="540" windowWidth="22260" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,6 +45,9 @@
     <t>1er_sustent</t>
   </si>
   <si>
+    <t>1er_lecciones</t>
+  </si>
+  <si>
     <t>1er_calif_final</t>
   </si>
   <si>
@@ -63,6 +66,9 @@
     <t>2do_sustent</t>
   </si>
   <si>
+    <t>2do_lecciones</t>
+  </si>
+  <si>
     <t>2do_calif_final</t>
   </si>
   <si>
@@ -75,6 +81,27 @@
     <t>2do_exam_tema3</t>
   </si>
   <si>
+    <t>2do_exam_tema4</t>
+  </si>
+  <si>
+    <t>2do_exam_tema5</t>
+  </si>
+  <si>
+    <t>2do_exam_tema6</t>
+  </si>
+  <si>
+    <t>2do_exam_tema7</t>
+  </si>
+  <si>
+    <t>2do_exam_tema8</t>
+  </si>
+  <si>
+    <t>2do_exam_tema9</t>
+  </si>
+  <si>
+    <t>2do_exam_tema10</t>
+  </si>
+  <si>
     <t>calif_final_practica</t>
   </si>
   <si>
@@ -97,40 +124,13 @@
   </si>
   <si>
     <t>Vacio/2/3</t>
-  </si>
-  <si>
-    <t>1er_lecciones</t>
-  </si>
-  <si>
-    <t>2do_lecciones</t>
-  </si>
-  <si>
-    <t>2do_exam_tema4</t>
-  </si>
-  <si>
-    <t>2do_exam_tema5</t>
-  </si>
-  <si>
-    <t>2do_exam_tema6</t>
-  </si>
-  <si>
-    <t>2do_exam_tema7</t>
-  </si>
-  <si>
-    <t>2do_exam_tema8</t>
-  </si>
-  <si>
-    <t>2do_exam_tema9</t>
-  </si>
-  <si>
-    <t>2do_exam_tema10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,20 +140,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -237,14 +223,14 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFF8E56"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FF000000"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFD8BF"/>
       </patternFill>
     </fill>
   </fills>
@@ -397,18 +383,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -431,78 +411,52 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -761,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -769,33 +723,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF1" sqref="AF1"/>
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="16.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="16.83203125" style="8" customWidth="1"/>
-    <col min="28" max="28" width="17.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="16.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" style="10" customWidth="1"/>
+    <col min="17" max="17" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="16.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="16.83203125" style="10" customWidth="1"/>
+    <col min="28" max="28" width="17.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="16.5" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1" ht="45.75" customHeight="1">
@@ -824,325 +778,219 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="5" t="s">
+      <c r="AB1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="5" t="s">
+      <c r="AC1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AD1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AE1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AF1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AG1" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="13">
+        <v>20</v>
+      </c>
+      <c r="H2" s="13">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>10</v>
+      </c>
+      <c r="J2" s="13">
+        <v>100</v>
+      </c>
+      <c r="K2" s="13">
+        <v>20</v>
+      </c>
+      <c r="L2" s="13">
+        <v>30</v>
+      </c>
+      <c r="M2" s="13">
+        <v>50</v>
+      </c>
+      <c r="N2" s="14">
+        <v>20</v>
+      </c>
+      <c r="O2" s="14">
+        <v>1</v>
+      </c>
+      <c r="P2" s="14">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>100</v>
+      </c>
+      <c r="R2" s="14">
+        <v>15</v>
+      </c>
+      <c r="S2" s="14">
+        <v>10</v>
+      </c>
+      <c r="T2" s="14">
+        <v>20</v>
+      </c>
+      <c r="U2" s="14">
+        <v>15</v>
+      </c>
+      <c r="V2" s="14">
+        <v>20</v>
+      </c>
+      <c r="W2" s="14">
+        <v>1</v>
+      </c>
+      <c r="X2" s="14">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="14">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="19">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="15">
+        <v>100</v>
+      </c>
+      <c r="AC2" s="16">
         <v>25</v>
       </c>
-      <c r="G2" s="20">
-        <v>20</v>
-      </c>
-      <c r="H2" s="20">
-        <v>1</v>
-      </c>
-      <c r="I2" s="20">
-        <v>10</v>
-      </c>
-      <c r="J2" s="20">
+      <c r="AD2" s="17">
         <v>100</v>
       </c>
-      <c r="K2" s="20">
-        <v>20</v>
-      </c>
-      <c r="L2" s="20">
-        <v>30</v>
-      </c>
-      <c r="M2" s="20">
+      <c r="AE2" s="17">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="17">
         <v>50</v>
       </c>
-      <c r="N2" s="21">
-        <v>20</v>
-      </c>
-      <c r="O2" s="21">
-        <v>1</v>
-      </c>
-      <c r="P2" s="21">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="21">
-        <v>100</v>
-      </c>
-      <c r="R2" s="21">
-        <v>15</v>
-      </c>
-      <c r="S2" s="21">
-        <v>10</v>
-      </c>
-      <c r="T2" s="21">
-        <v>20</v>
-      </c>
-      <c r="U2" s="21">
-        <v>15</v>
-      </c>
-      <c r="V2" s="21">
-        <v>20</v>
-      </c>
-      <c r="W2" s="21">
-        <v>1</v>
-      </c>
-      <c r="X2" s="21">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="21">
-        <v>9</v>
-      </c>
-      <c r="AA2" s="26">
-        <v>10</v>
-      </c>
-      <c r="AB2" s="22">
-        <v>100</v>
-      </c>
-      <c r="AC2" s="23">
-        <v>25</v>
-      </c>
-      <c r="AD2" s="24">
-        <v>100</v>
-      </c>
-      <c r="AE2" s="24">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="24">
-        <v>50</v>
-      </c>
-      <c r="AG2" s="25">
+      <c r="AG2" s="18">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:33">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-    </row>
-    <row r="4" spans="1:33">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-    </row>
-    <row r="5" spans="1:33">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="12"/>
-    </row>
-    <row r="6" spans="1:33">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>